<commit_message>
SPER et analyse de risque
</commit_message>
<xml_diff>
--- a/04 - Analyse & Conception/Listes_E_S_UsineDeTri_PRI_PROJET-IEC61499_V0_1.xlsx
+++ b/04 - Analyse & Conception/Listes_E_S_UsineDeTri_PRI_PROJET-IEC61499_V0_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damienlorigeon/Documents/Polytech/5A/PRI/PRI-IEC61499-UniversalAutomation/04 - Analyse &amp; Conception/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC344162-0F39-BC47-BCBB-FF78364B9046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EFE9CC-8735-434E-9064-679F49A3D724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="620" windowWidth="28040" windowHeight="15740" xr2:uid="{615C8FA3-7A25-874E-8DE4-B37DBC7D11AC}"/>
+    <workbookView xWindow="380" yWindow="620" windowWidth="28040" windowHeight="15740" activeTab="1" xr2:uid="{615C8FA3-7A25-874E-8DE4-B37DBC7D11AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Capteurs" sheetId="1" r:id="rId1"/>
@@ -662,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020B4BA0-8418-724D-B521-29CFB398DE99}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A786B6-0A41-7847-ACE2-12627EEEC095}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
-      <selection activeCell="A16" sqref="A5:A16"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>